<commit_message>
functions to add singlecell object
</commit_message>
<xml_diff>
--- a/data/masterseq_app/template.xlsx
+++ b/data/masterseq_app/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frank/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuxinli/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26B29B7-2027-2845-8257-AA2B098DB36D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709DE89A-DB51-C742-A5DE-220022FCE24C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="580" windowWidth="40960" windowHeight="22460" activeTab="1" xr2:uid="{0BA43C7A-E819-E44A-BC5D-1B0EA814106C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" xr2:uid="{0BA43C7A-E819-E44A-BC5D-1B0EA814106C}"/>
   </bookViews>
   <sheets>
     <sheet name="samples" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="99">
   <si>
     <t>From sample submission form</t>
   </si>
@@ -318,6 +318,15 @@
   </si>
   <si>
     <t>10xATAC</t>
+  </si>
+  <si>
+    <t>Project number</t>
+  </si>
+  <si>
+    <t>Task number</t>
+  </si>
+  <si>
+    <t>Funding Source Number (if sponsored research)</t>
   </si>
 </sst>
 </file>
@@ -819,11 +828,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F7609B9-C4B6-F14F-A209-FF45D69C71CA}">
-  <dimension ref="A1:Y2"/>
+  <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -835,24 +842,27 @@
     <col min="6" max="6" width="17.33203125" customWidth="1"/>
     <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.6640625" customWidth="1"/>
-    <col min="10" max="10" width="46.33203125" customWidth="1"/>
-    <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="13.83203125" customWidth="1"/>
-    <col min="13" max="13" width="14.83203125" customWidth="1"/>
-    <col min="15" max="15" width="11.1640625" customWidth="1"/>
-    <col min="17" max="17" width="13.6640625" customWidth="1"/>
-    <col min="18" max="18" width="13.5" customWidth="1"/>
-    <col min="19" max="19" width="14.1640625" customWidth="1"/>
-    <col min="20" max="20" width="13.33203125" customWidth="1"/>
-    <col min="21" max="21" width="45.1640625" customWidth="1"/>
+    <col min="9" max="9" width="15.5" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" customWidth="1"/>
+    <col min="11" max="11" width="23.33203125" customWidth="1"/>
+    <col min="12" max="12" width="32.6640625" customWidth="1"/>
+    <col min="13" max="13" width="46.33203125" customWidth="1"/>
+    <col min="14" max="14" width="12" customWidth="1"/>
+    <col min="15" max="15" width="13.83203125" customWidth="1"/>
+    <col min="16" max="16" width="14.83203125" customWidth="1"/>
+    <col min="18" max="18" width="11.1640625" customWidth="1"/>
+    <col min="20" max="20" width="13.6640625" customWidth="1"/>
+    <col min="21" max="21" width="13.5" customWidth="1"/>
     <col min="22" max="22" width="14.1640625" customWidth="1"/>
-    <col min="23" max="23" width="14" customWidth="1"/>
-    <col min="24" max="24" width="11.83203125" customWidth="1"/>
-    <col min="25" max="25" width="43.33203125" customWidth="1"/>
+    <col min="23" max="23" width="13.33203125" customWidth="1"/>
+    <col min="24" max="24" width="45.1640625" customWidth="1"/>
+    <col min="25" max="25" width="14.1640625" customWidth="1"/>
+    <col min="26" max="26" width="14" customWidth="1"/>
+    <col min="27" max="27" width="11.83203125" customWidth="1"/>
+    <col min="28" max="28" width="43.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -875,15 +885,18 @@
       <c r="R1" s="3"/>
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="6" t="s">
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="8"/>
-    </row>
-    <row r="2" spans="1:25" ht="46" x14ac:dyDescent="0.2">
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
+      <c r="AB1" s="8"/>
+    </row>
+    <row r="2" spans="1:28" ht="61" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
@@ -908,61 +921,70 @@
       <c r="H2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="L2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="M2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="N2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="R2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="S2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="10" t="s">
+      <c r="T2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="10" t="s">
+      <c r="U2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="S2" s="10" t="s">
+      <c r="V2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="T2" s="10" t="s">
+      <c r="W2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="X2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="V2" s="10" t="s">
+      <c r="Y2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="W2" s="10" t="s">
+      <c r="Z2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="X2" s="10" t="s">
+      <c r="AA2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="Y2" s="9" t="s">
+      <c r="AB2" s="9" t="s">
         <v>94</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A1048576 V3:V1048576" xr:uid="{2E778634-3350-3242-8614-54899DD376E9}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A1048576 Y3:Y1048576" xr:uid="{2E778634-3350-3242-8614-54899DD376E9}">
       <formula1>42736</formula1>
     </dataValidation>
   </dataValidations>
@@ -974,61 +996,61 @@
           <x14:formula1>
             <xm:f>samples_validation!$B$2:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>L3:L1048576</xm:sqref>
+          <xm:sqref>O3:O1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{037BAEAE-C9B6-AC49-AEB7-DF096E2D6AE0}">
           <x14:formula1>
             <xm:f>samples_validation!$C$2:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>M3:M1048576</xm:sqref>
+          <xm:sqref>P3:P1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{10BC871A-5950-0E45-93D0-7E38F0D7C026}">
           <x14:formula1>
             <xm:f>samples_validation!$D$2:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>N3:N1048576</xm:sqref>
+          <xm:sqref>Q3:Q1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E5A825B7-A366-5E42-ABD7-4A1AC5B7146B}">
           <x14:formula1>
             <xm:f>samples_validation!$E$2:$E$5</xm:f>
           </x14:formula1>
-          <xm:sqref>P3:P1048576</xm:sqref>
+          <xm:sqref>S3:S1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DC3A8C2C-589E-3240-9C4B-BC72A706DBB1}">
           <x14:formula1>
             <xm:f>samples_validation!$F$2:$F$7</xm:f>
           </x14:formula1>
-          <xm:sqref>Q3:Q1048576</xm:sqref>
+          <xm:sqref>T3:T1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{574E566B-1CD4-9344-89A3-2047F0AFE019}">
           <x14:formula1>
             <xm:f>samples_validation!$G$2:$G$3</xm:f>
           </x14:formula1>
-          <xm:sqref>R3:R1048576</xm:sqref>
+          <xm:sqref>U3:U1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A7E06BF9-B69C-0443-9D53-F74897CB1E9B}">
           <x14:formula1>
             <xm:f>samples_validation!$I$2:$I$5</xm:f>
           </x14:formula1>
-          <xm:sqref>T3:T1048576</xm:sqref>
+          <xm:sqref>W3:W1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FE302A98-9A3D-1342-B6E0-51306F068905}">
           <x14:formula1>
             <xm:f>samples_validation!$H$2:$H$3</xm:f>
           </x14:formula1>
-          <xm:sqref>S3:S1048576</xm:sqref>
+          <xm:sqref>V3:V1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AACF20CC-1108-2D46-A0E1-66CEFABE5D1A}">
           <x14:formula1>
             <xm:f>samples_validation!$J$2:$J$4</xm:f>
           </x14:formula1>
-          <xm:sqref>X3:X1048576</xm:sqref>
+          <xm:sqref>AA3:AA1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FE30D4AF-4A47-1240-A444-C0EDDC356808}">
           <x14:formula1>
             <xm:f>samples_validation!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>K3:K1048576</xm:sqref>
+          <xm:sqref>N3:N1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1040,7 +1062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95FDDB9A-F01E-4849-87EC-00E3C8EFF76F}">
   <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add the financial unit in the template exel file
</commit_message>
<xml_diff>
--- a/data/masterseq_app/template.xlsx
+++ b/data/masterseq_app/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuxinli/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurenthomas/Dropbox (UCSD_Epigenomics)/working, ideas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709DE89A-DB51-C742-A5DE-220022FCE24C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455CE325-275F-9940-AFBD-A088EC3EC9D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" xr2:uid="{0BA43C7A-E819-E44A-BC5D-1B0EA814106C}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="libraries_validation" sheetId="4" r:id="rId5"/>
     <sheet name="sequencings_validation" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="181029" calcOnSave="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="100">
   <si>
     <t>From sample submission form</t>
   </si>
@@ -327,6 +327,9 @@
   </si>
   <si>
     <t>Funding Source Number (if sponsored research)</t>
+  </si>
+  <si>
+    <t>Financial Unit</t>
   </si>
 </sst>
 </file>
@@ -828,9 +831,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F7609B9-C4B6-F14F-A209-FF45D69C71CA}">
-  <dimension ref="A1:AB2"/>
+  <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -842,27 +847,28 @@
     <col min="6" max="6" width="17.33203125" customWidth="1"/>
     <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" customWidth="1"/>
-    <col min="11" max="11" width="23.33203125" customWidth="1"/>
-    <col min="12" max="12" width="32.6640625" customWidth="1"/>
-    <col min="13" max="13" width="46.33203125" customWidth="1"/>
-    <col min="14" max="14" width="12" customWidth="1"/>
-    <col min="15" max="15" width="13.83203125" customWidth="1"/>
-    <col min="16" max="16" width="14.83203125" customWidth="1"/>
-    <col min="18" max="18" width="11.1640625" customWidth="1"/>
-    <col min="20" max="20" width="13.6640625" customWidth="1"/>
-    <col min="21" max="21" width="13.5" customWidth="1"/>
-    <col min="22" max="22" width="14.1640625" customWidth="1"/>
-    <col min="23" max="23" width="13.33203125" customWidth="1"/>
-    <col min="24" max="24" width="45.1640625" customWidth="1"/>
-    <col min="25" max="25" width="14.1640625" customWidth="1"/>
-    <col min="26" max="26" width="14" customWidth="1"/>
-    <col min="27" max="27" width="11.83203125" customWidth="1"/>
-    <col min="28" max="28" width="43.33203125" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" customWidth="1"/>
+    <col min="10" max="10" width="15.5" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="23.33203125" customWidth="1"/>
+    <col min="13" max="13" width="32.6640625" customWidth="1"/>
+    <col min="14" max="14" width="46.33203125" customWidth="1"/>
+    <col min="15" max="15" width="12" customWidth="1"/>
+    <col min="16" max="16" width="13.83203125" customWidth="1"/>
+    <col min="17" max="17" width="14.83203125" customWidth="1"/>
+    <col min="19" max="19" width="11.1640625" customWidth="1"/>
+    <col min="21" max="21" width="13.6640625" customWidth="1"/>
+    <col min="22" max="22" width="13.5" customWidth="1"/>
+    <col min="23" max="23" width="14.1640625" customWidth="1"/>
+    <col min="24" max="24" width="13.33203125" customWidth="1"/>
+    <col min="25" max="25" width="45.1640625" customWidth="1"/>
+    <col min="26" max="26" width="14.1640625" customWidth="1"/>
+    <col min="27" max="27" width="14" customWidth="1"/>
+    <col min="28" max="28" width="11.83203125" customWidth="1"/>
+    <col min="29" max="29" width="43.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -888,15 +894,16 @@
       <c r="U1" s="3"/>
       <c r="V1" s="3"/>
       <c r="W1" s="3"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="6" t="s">
+      <c r="X1" s="3"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="Z1" s="7"/>
       <c r="AA1" s="7"/>
-      <c r="AB1" s="8"/>
-    </row>
-    <row r="2" spans="1:28" ht="61" x14ac:dyDescent="0.2">
+      <c r="AB1" s="7"/>
+      <c r="AC1" s="8"/>
+    </row>
+    <row r="2" spans="1:29" ht="46" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
@@ -922,69 +929,72 @@
         <v>9</v>
       </c>
       <c r="I2" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="L2" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="M2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="N2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="R2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="10" t="s">
+      <c r="S2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="T2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="10" t="s">
+      <c r="U2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="U2" s="10" t="s">
+      <c r="V2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="V2" s="10" t="s">
+      <c r="W2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="W2" s="10" t="s">
+      <c r="X2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="X2" s="9" t="s">
+      <c r="Y2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="Y2" s="10" t="s">
+      <c r="Z2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="Z2" s="10" t="s">
+      <c r="AA2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="AA2" s="10" t="s">
+      <c r="AB2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="AB2" s="9" t="s">
+      <c r="AC2" s="9" t="s">
         <v>94</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A1048576 Y3:Y1048576" xr:uid="{2E778634-3350-3242-8614-54899DD376E9}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A1048576 Z3:Z1048576" xr:uid="{2E778634-3350-3242-8614-54899DD376E9}">
       <formula1>42736</formula1>
     </dataValidation>
   </dataValidations>
@@ -996,61 +1006,61 @@
           <x14:formula1>
             <xm:f>samples_validation!$B$2:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>O3:O1048576</xm:sqref>
+          <xm:sqref>P3:P1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{037BAEAE-C9B6-AC49-AEB7-DF096E2D6AE0}">
           <x14:formula1>
             <xm:f>samples_validation!$C$2:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>P3:P1048576</xm:sqref>
+          <xm:sqref>Q3:Q1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{10BC871A-5950-0E45-93D0-7E38F0D7C026}">
           <x14:formula1>
             <xm:f>samples_validation!$D$2:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>Q3:Q1048576</xm:sqref>
+          <xm:sqref>R3:R1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E5A825B7-A366-5E42-ABD7-4A1AC5B7146B}">
           <x14:formula1>
             <xm:f>samples_validation!$E$2:$E$5</xm:f>
           </x14:formula1>
-          <xm:sqref>S3:S1048576</xm:sqref>
+          <xm:sqref>T3:T1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DC3A8C2C-589E-3240-9C4B-BC72A706DBB1}">
           <x14:formula1>
             <xm:f>samples_validation!$F$2:$F$7</xm:f>
           </x14:formula1>
-          <xm:sqref>T3:T1048576</xm:sqref>
+          <xm:sqref>U3:U1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{574E566B-1CD4-9344-89A3-2047F0AFE019}">
           <x14:formula1>
             <xm:f>samples_validation!$G$2:$G$3</xm:f>
           </x14:formula1>
-          <xm:sqref>U3:U1048576</xm:sqref>
+          <xm:sqref>V3:V1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A7E06BF9-B69C-0443-9D53-F74897CB1E9B}">
           <x14:formula1>
             <xm:f>samples_validation!$I$2:$I$5</xm:f>
           </x14:formula1>
-          <xm:sqref>W3:W1048576</xm:sqref>
+          <xm:sqref>X3:X1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FE302A98-9A3D-1342-B6E0-51306F068905}">
           <x14:formula1>
             <xm:f>samples_validation!$H$2:$H$3</xm:f>
           </x14:formula1>
-          <xm:sqref>V3:V1048576</xm:sqref>
+          <xm:sqref>W3:W1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AACF20CC-1108-2D46-A0E1-66CEFABE5D1A}">
           <x14:formula1>
             <xm:f>samples_validation!$J$2:$J$4</xm:f>
           </x14:formula1>
-          <xm:sqref>AA3:AA1048576</xm:sqref>
+          <xm:sqref>AB3:AB1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FE30D4AF-4A47-1240-A444-C0EDDC356808}">
           <x14:formula1>
             <xm:f>samples_validation!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>N3:N1048576</xm:sqref>
+          <xm:sqref>O3:O1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>